<commit_message>
Included graphs in README.md
</commit_message>
<xml_diff>
--- a/graphs/algorithm-results.xlsx
+++ b/graphs/algorithm-results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/njblanch_uvm_edu/Documents/CS 124/Homework/Project4-njblanch/graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0151F664-7407-104A-B60E-112C0BE39FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{293E2D2F-DFDD-7E42-ABC0-B3696252AF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
@@ -5762,8 +5762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="262" zoomScaleNormal="262" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>